<commit_message>
Added test script for add new role- administrator, Updated framework with page-objects. Added Locators of new role-setting page. Added methods to add new role
</commit_message>
<xml_diff>
--- a/Test_Data/Test_Data.xlsx
+++ b/Test_Data/Test_Data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ManishaDrive1\PrimeBPM\primeBPM\primeBPM\Test_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -57,20 +52,20 @@
     <t>No</t>
   </si>
   <si>
-    <t>https://www.primebpmapp.com/ioadmin/</t>
-  </si>
-  <si>
-    <t>manisha@vtestcorp.com</t>
-  </si>
-  <si>
-    <t>Manisha1!</t>
+    <t>saumyata@vtestcorp.com</t>
+  </si>
+  <si>
+    <t>Saumyata2!</t>
+  </si>
+  <si>
+    <t>https://www.primebpmapp.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -490,41 +485,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="18.33203125"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="D4" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -532,42 +527,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="2"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -576,14 +572,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -595,12 +591,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -612,25 +608,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="24.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -653,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="24.75" customHeight="1">
       <c r="B3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update #A-2 - Test cases No. 2  -"User should be able to insert Roles through Admin (Settings) page by uploading Excel Templates" - 50% done
</commit_message>
<xml_diff>
--- a/Test_Data/Test_Data.xlsx
+++ b/Test_Data/Test_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>URL</t>
   </si>
@@ -59,12 +59,28 @@
   </si>
   <si>
     <t>https://www.primebpmapp.com/</t>
+  </si>
+  <si>
+    <t>Testatlsr7pVN3</t>
+  </si>
+  <si>
+    <t>TestkrF7ig94jY</t>
+  </si>
+  <si>
+    <t>Test91ycjxveFT</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>TestqRHrmRD2PW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -501,11 +517,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.33203125"/>
-    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="18.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="52.5546875" collapsed="true"/>
+    <col min="5" max="1025" width="8.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -617,13 +633,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" hidden="true" width="28.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" hidden="true" width="9.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="24.75" customHeight="1">
@@ -655,6 +671,9 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added send approval serial & parallel cycle desinger test scripts
</commit_message>
<xml_diff>
--- a/Test_Data/Test_Data.xlsx
+++ b/Test_Data/Test_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>URL</t>
   </si>
@@ -61,27 +61,23 @@
     <t>https://www.primebpmapp.com/</t>
   </si>
   <si>
-    <t>Testatlsr7pVN3</t>
-  </si>
-  <si>
-    <t>TestkrF7ig94jY</t>
-  </si>
-  <si>
-    <t>Test91ycjxveFT</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>TestqRHrmRD2PW</t>
+  </si>
+  <si>
+    <t>Valid User PA Name</t>
+  </si>
+  <si>
+    <t>testuserpa@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -109,6 +105,11 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Prime"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,13 +154,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -509,19 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D13"/>
+  <dimension ref="A3:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="52.5546875" collapsed="true"/>
-    <col min="5" max="1025" width="8.5546875" collapsed="true"/>
+    <col min="1" max="1" width="18.33203125" collapsed="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="52.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="8.5546875" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -555,7 +557,15 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="C9" s="4"/>
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="2"/>
@@ -577,9 +587,10 @@
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -625,7 +636,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -633,13 +644,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="32.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" hidden="true" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" hidden="true" width="9.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.33203125" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.109375" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="24.75" customHeight="1">
@@ -673,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added publish process map after approval test script in collaboration
</commit_message>
<xml_diff>
--- a/Test_Data/Test_Data.xlsx
+++ b/Test_Data/Test_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>URL</t>
   </si>
@@ -67,17 +67,20 @@
     <t>Valid User PA Name</t>
   </si>
   <si>
+    <t>Test@123</t>
+  </si>
+  <si>
     <t>testuserpa@gmail.com</t>
   </si>
   <si>
-    <t>Test@123</t>
+    <t>pauser@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,11 +108,6 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF222222"/>
-      <name val="Prime"/>
     </font>
   </fonts>
   <fills count="3">
@@ -154,14 +152,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -503,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,7 +511,7 @@
   <dimension ref="A3:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -560,16 +557,23 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="1"/>
@@ -588,9 +592,12 @@
     <hyperlink ref="B8" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>